<commit_message>
Removed some spaces from the employee names
</commit_message>
<xml_diff>
--- a/Database Scripts/EmployeeData.xlsx
+++ b/Database Scripts/EmployeeData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03_Code\04_GitHub\EmployeeManagement\Database Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7CDD0F-105E-497B-93DD-F342A1C20006}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D10FB1-D6DF-4B46-8E45-834F22B3C365}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{DE7B9934-B2E9-4ED0-8D96-58F9AC0C3B47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
   <si>
     <t>first_name</t>
   </si>
@@ -162,33 +161,18 @@
     <t>410-655-8723</t>
   </si>
   <si>
-    <t>Bruce </t>
-  </si>
-  <si>
     <t>Wayne</t>
   </si>
   <si>
-    <t>Tony </t>
-  </si>
-  <si>
     <t>Stark</t>
   </si>
   <si>
-    <t>Clark </t>
-  </si>
-  <si>
     <t>Kent</t>
   </si>
   <si>
-    <t>Barry </t>
-  </si>
-  <si>
     <t>Allen</t>
   </si>
   <si>
-    <t>Steve </t>
-  </si>
-  <si>
     <t>Rogers</t>
   </si>
   <si>
@@ -231,15 +215,9 @@
     <t>F</t>
   </si>
   <si>
-    <t>Selina </t>
-  </si>
-  <si>
     <t>Kyle</t>
   </si>
   <si>
-    <t>Natasha </t>
-  </si>
-  <si>
     <t>Romanova</t>
   </si>
   <si>
@@ -280,6 +258,24 @@
   </si>
   <si>
     <t>AUS</t>
+  </si>
+  <si>
+    <t>Selina</t>
+  </si>
+  <si>
+    <t>Tony</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Barry</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Natasha</t>
   </si>
 </sst>
 </file>
@@ -634,12 +630,12 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.81640625" customWidth="1"/>
     <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.90625" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
@@ -647,7 +643,7 @@
     <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="42.453125" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" customWidth="1"/>
     <col min="11" max="11" width="25.81640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.6328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
@@ -685,7 +681,7 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -699,7 +695,7 @@
         <v>9000</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -708,17 +704,17 @@
         <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K2" t="str">
-        <f>_xlfn.CONCAT(LOWER(A2),".",LOWER(B2),"@",J2)</f>
+        <f>CONCATENATE(LOWER(A2),".",LOWER(B2),"@",J2)</f>
         <v>mickey.mouse@gmail.com</v>
       </c>
       <c r="L2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -732,7 +728,7 @@
         <v>9000</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
         <v>34</v>
@@ -741,17 +737,17 @@
         <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K16" si="0">_xlfn.CONCAT(LOWER(A3),".",LOWER(B3),"@",J3)</f>
+        <f t="shared" ref="K3:K16" si="0">CONCATENATE(LOWER(A3),".",LOWER(B3),"@",J3)</f>
         <v>donald.duck@hotmail.com</v>
       </c>
       <c r="L3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -765,7 +761,7 @@
         <v>9000</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="H4" t="s">
         <v>35</v>
@@ -774,22 +770,22 @@
         <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="0"/>
         <v>scrooge.mcduck@aol.com</v>
       </c>
       <c r="L4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -798,7 +794,7 @@
         <v>9000</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
@@ -807,17 +803,17 @@
         <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
         <v>daisy.duck@aol.com</v>
       </c>
       <c r="L5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M5" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -831,7 +827,7 @@
         <v>5000</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -843,17 +839,17 @@
         <v>27</v>
       </c>
       <c r="J6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
         <v>snow.white@aol.com</v>
       </c>
       <c r="L6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -867,7 +863,7 @@
         <v>5000</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -879,17 +875,17 @@
         <v>28</v>
       </c>
       <c r="J7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
         <v>daffy.duck@hotmail.com</v>
       </c>
       <c r="L7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -903,7 +899,7 @@
         <v>5000</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
@@ -915,17 +911,17 @@
         <v>29</v>
       </c>
       <c r="J8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
         <v>bugs.bunny@hotmail.com</v>
       </c>
       <c r="L8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -939,10 +935,10 @@
         <v>5000</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
         <v>40</v>
@@ -951,34 +947,34 @@
         <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
         <v>buzz.lightyear@gmail.com</v>
       </c>
       <c r="L9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C10">
         <v>5000</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H10" t="s">
         <v>41</v>
@@ -987,34 +983,34 @@
         <v>31</v>
       </c>
       <c r="J10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
-        <v>selina .kyle@aol.com</v>
+        <v>selina.kyle@aol.com</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M10" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
         <v>43</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
       </c>
       <c r="C11">
         <v>5000</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -1023,210 +1019,201 @@
         <v>32</v>
       </c>
       <c r="J11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>bruce .wayne@gmail.com</v>
+        <v>bruce.wayne@gmail.com</v>
       </c>
       <c r="L11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M11" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12">
         <v>2000</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
-        <v>tony .stark@gmail.com</v>
+        <v>tony.stark@gmail.com</v>
       </c>
       <c r="L12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M12" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C13">
         <v>2000</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s">
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" t="s">
         <v>58</v>
-      </c>
-      <c r="J13" t="s">
-        <v>63</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
-        <v>clark .kent@aol.com</v>
+        <v>clark.kent@aol.com</v>
       </c>
       <c r="L13" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C14">
         <v>2000</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
       </c>
       <c r="H14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
-        <v>barry .allen@gmail.com</v>
+        <v>barry.allen@gmail.com</v>
       </c>
       <c r="L14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M14" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C15">
         <v>1000</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F15" t="s">
         <v>18</v>
       </c>
       <c r="H15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" t="s">
         <v>56</v>
-      </c>
-      <c r="I15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" t="s">
-        <v>61</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
-        <v>steve .rogers@gmail.com</v>
+        <v>steve.rogers@gmail.com</v>
       </c>
       <c r="L15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="M15" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C16">
         <v>1000</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="I16" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="J16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
-        <v>natasha .romanova@aol.com</v>
+        <v>natasha.romanova@aol.com</v>
       </c>
       <c r="L16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M16" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A11" r:id="rId1" display="https://www.sheknows.com/baby-names/name/bruce" xr:uid="{C02ACCAD-EC2F-4797-B3F8-140A7D9A4123}"/>
-    <hyperlink ref="A12" r:id="rId2" display="https://www.sheknows.com/baby-names/name/tony" xr:uid="{3FC7D1B6-C90F-48D8-98C8-96C2B8658B5C}"/>
-    <hyperlink ref="A13" r:id="rId3" display="https://www.sheknows.com/baby-names/name/clark" xr:uid="{840CBBA7-36F1-4F1F-BBC4-0DC81BB18C48}"/>
-    <hyperlink ref="A14" r:id="rId4" display="https://www.sheknows.com/baby-names/name/barry" xr:uid="{76B40D47-638E-4EEB-891C-9FA775B68363}"/>
-    <hyperlink ref="A15" r:id="rId5" display="https://www.sheknows.com/baby-names/name/steve" xr:uid="{1C9CF949-5A09-46D8-A978-8DD571E9BC28}"/>
-    <hyperlink ref="A10" r:id="rId6" display="https://www.sheknows.com/baby-names/name/selina" xr:uid="{801681E0-9DB3-41DB-9375-ABC038D13145}"/>
-    <hyperlink ref="A16" r:id="rId7" display="https://www.sheknows.com/baby-names/name/natasha" xr:uid="{B7248AA6-6C07-4E86-B6C6-3EDB4DB77146}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>